<commit_message>
fix list of forms and excel samples
</commit_message>
<xml_diff>
--- a/data/Excel/1.1.xlsx
+++ b/data/Excel/1.1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bkl\source\repos\repo\RAO_Project\data\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\RAO_Project\data\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2163F1A6-8237-4529-8A9A-310B47E6EE6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1.0" sheetId="3" r:id="rId1"/>
@@ -194,9 +195,6 @@
     <t>Дата окончания предыдущего отчетного периода</t>
   </si>
   <si>
-    <t>Дата окончания настящего отчетного периода</t>
-  </si>
-  <si>
     <t>Номер корректировки</t>
   </si>
   <si>
@@ -300,12 +298,15 @@
   </si>
   <si>
     <t>Право собственности на ЗРИ</t>
+  </si>
+  <si>
+    <t>Дата окончания настоящего отчетного периода</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -849,7 +850,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -921,125 +922,194 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1071,9 +1141,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1082,90 +1149,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="1"/>
-    <cellStyle name="Обычный 3" xfId="2"/>
+    <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Обычный 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1442,397 +1431,397 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="55" zoomScaleNormal="100" zoomScaleSheetLayoutView="55" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A11" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="37.42578125" style="1" customWidth="1"/>
-    <col min="7" max="9" width="10.5703125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="16.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="37.453125" style="1" customWidth="1"/>
+    <col min="7" max="9" width="10.54296875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I1" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="48" t="s">
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-    </row>
-    <row r="4" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+    </row>
+    <row r="4" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-    </row>
-    <row r="5" spans="1:9" ht="2.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-    </row>
-    <row r="6" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="80"/>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="80"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+    </row>
+    <row r="5" spans="1:9" ht="2.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+    </row>
+    <row r="6" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D6" s="11"/>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="32"/>
+      <c r="F6" s="30"/>
       <c r="G6" s="10" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
+    <row r="9" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="42" t="s">
+      <c r="B10" s="77"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="75" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+    <row r="11" spans="1:9" ht="86.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="42"/>
-    </row>
-    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="75"/>
+    </row>
+    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="42"/>
-    </row>
-    <row r="13" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="42"/>
-    </row>
-    <row r="14" spans="1:9" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="42"/>
-    </row>
-    <row r="15" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="s">
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="71"/>
+      <c r="F12" s="75"/>
+    </row>
+    <row r="13" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="69"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="75"/>
+    </row>
+    <row r="14" spans="1:9" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="72"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="75"/>
+    </row>
+    <row r="15" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="98"/>
-      <c r="G15" s="99"/>
-      <c r="H15" s="99"/>
-      <c r="I15" s="89"/>
-    </row>
-    <row r="16" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="41"/>
+    </row>
+    <row r="16" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="B16" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="95"/>
-      <c r="F16" s="100"/>
-      <c r="G16" s="93"/>
-      <c r="H16" s="93"/>
-      <c r="I16" s="90"/>
-    </row>
-    <row r="17" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
-      <c r="B17" s="54" t="s">
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="35"/>
+    </row>
+    <row r="17" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="48"/>
+      <c r="B17" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="93"/>
-      <c r="H17" s="93"/>
-      <c r="I17" s="90"/>
-    </row>
-    <row r="18" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
-      <c r="B18" s="54" t="s">
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="35"/>
+    </row>
+    <row r="18" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="48"/>
+      <c r="B18" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="100"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
-      <c r="I18" s="90"/>
-    </row>
-    <row r="19" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
-      <c r="B19" s="54" t="s">
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="35"/>
+    </row>
+    <row r="19" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="48"/>
+      <c r="B19" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="93"/>
-      <c r="H19" s="93"/>
-      <c r="I19" s="90"/>
-    </row>
-    <row r="20" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
-      <c r="B20" s="54" t="s">
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="35"/>
+    </row>
+    <row r="20" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="48"/>
+      <c r="B20" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="64"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="93"/>
-      <c r="H20" s="93"/>
-      <c r="I20" s="90"/>
-    </row>
-    <row r="21" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="54" t="s">
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="35"/>
+    </row>
+    <row r="21" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="48"/>
+      <c r="B21" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="93"/>
-      <c r="H21" s="93"/>
-      <c r="I21" s="90"/>
-    </row>
-    <row r="22" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
-      <c r="B22" s="55" t="s">
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="35"/>
+    </row>
+    <row r="22" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="48"/>
+      <c r="B22" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="100"/>
-      <c r="G22" s="93"/>
-      <c r="H22" s="93"/>
-      <c r="I22" s="90"/>
-    </row>
-    <row r="23" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="51"/>
-      <c r="B23" s="55" t="s">
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="35"/>
+    </row>
+    <row r="23" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="48"/>
+      <c r="B23" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="100"/>
-      <c r="G23" s="93"/>
-      <c r="H23" s="93"/>
-      <c r="I23" s="90"/>
-    </row>
-    <row r="24" spans="1:9" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="52"/>
-      <c r="B24" s="59" t="s">
+      <c r="C23" s="54"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="35"/>
+    </row>
+    <row r="24" spans="1:9" ht="23.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="66"/>
+      <c r="B24" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="96"/>
-      <c r="F24" s="102"/>
-      <c r="G24" s="103"/>
-      <c r="H24" s="103"/>
-      <c r="I24" s="92"/>
-    </row>
-    <row r="25" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="60" t="s">
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="38"/>
+    </row>
+    <row r="25" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="62" t="s">
+      <c r="B25" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="104"/>
-      <c r="G25" s="105"/>
-      <c r="H25" s="105"/>
-      <c r="I25" s="106"/>
-    </row>
-    <row r="26" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="51"/>
-      <c r="B26" s="54" t="s">
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="60"/>
+    </row>
+    <row r="26" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="48"/>
+      <c r="B26" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="64"/>
-      <c r="F26" s="101"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="91"/>
-    </row>
-    <row r="27" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="51"/>
-      <c r="B27" s="54" t="s">
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="62"/>
+    </row>
+    <row r="27" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="48"/>
+      <c r="B27" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="101"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54"/>
-      <c r="I27" s="91"/>
-    </row>
-    <row r="28" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="51"/>
-      <c r="B28" s="54" t="s">
+      <c r="C27" s="52"/>
+      <c r="D27" s="52"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="62"/>
+    </row>
+    <row r="28" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="48"/>
+      <c r="B28" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="91"/>
-    </row>
-    <row r="29" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="51"/>
-      <c r="B29" s="54" t="s">
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="62"/>
+    </row>
+    <row r="29" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="48"/>
+      <c r="B29" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="54"/>
-      <c r="D29" s="54"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="101"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="54"/>
-      <c r="I29" s="91"/>
-    </row>
-    <row r="30" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="51"/>
-      <c r="B30" s="55" t="s">
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="52"/>
+      <c r="I29" s="62"/>
+    </row>
+    <row r="30" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="48"/>
+      <c r="B30" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="100"/>
-      <c r="G30" s="93"/>
-      <c r="H30" s="93"/>
-      <c r="I30" s="90"/>
-    </row>
-    <row r="31" spans="1:9" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="51"/>
-      <c r="B31" s="55" t="s">
+      <c r="C30" s="54"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="35"/>
+    </row>
+    <row r="31" spans="1:9" ht="23.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="48"/>
+      <c r="B31" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="100"/>
-      <c r="G31" s="93"/>
-      <c r="H31" s="93"/>
-      <c r="I31" s="90"/>
-    </row>
-    <row r="32" spans="1:9" ht="23.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="61"/>
-      <c r="B32" s="66" t="s">
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="35"/>
+    </row>
+    <row r="32" spans="1:9" ht="23.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="49"/>
+      <c r="B32" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="66"/>
-      <c r="D32" s="66"/>
-      <c r="E32" s="97"/>
-      <c r="F32" s="102"/>
-      <c r="G32" s="103"/>
-      <c r="H32" s="103"/>
-      <c r="I32" s="92"/>
-    </row>
-    <row r="33" spans="1:9" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="38"/>
+    </row>
+    <row r="33" spans="1:9" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G33" s="9"/>
     </row>
-    <row r="34" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="56" t="s">
+    <row r="34" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B34" s="57"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="57"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="57"/>
-      <c r="G34" s="57"/>
-      <c r="H34" s="57"/>
-      <c r="I34" s="58"/>
-    </row>
-    <row r="35" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="43"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="43"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="44"/>
+    </row>
+    <row r="35" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="4"/>
       <c r="B35" s="3" t="s">
         <v>9</v>
@@ -1859,7 +1848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="2" customFormat="1" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" s="2" customFormat="1" ht="47" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="8" t="s">
         <v>1</v>
       </c>
@@ -1872,7 +1861,7 @@
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:9" s="2" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" s="2" customFormat="1" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="5" t="s">
         <v>0</v>
       </c>
@@ -1887,19 +1876,23 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="F32:I32"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F22:I22"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="F18:I18"/>
-    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="A12:E14"/>
+    <mergeCell ref="F10:F14"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A16:A24"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B23:E23"/>
     <mergeCell ref="A34:I34"/>
     <mergeCell ref="B24:E24"/>
     <mergeCell ref="A25:A32"/>
@@ -1916,90 +1909,86 @@
     <mergeCell ref="F27:I27"/>
     <mergeCell ref="F28:I28"/>
     <mergeCell ref="F29:I29"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A16:A24"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="A12:E14"/>
-    <mergeCell ref="F10:F14"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F19:I19"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="F32:I32"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F22:I22"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="53" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="52" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:W19"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="55" zoomScaleNormal="120" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7:O8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="120" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="10.5703125" style="13" customWidth="1"/>
-    <col min="6" max="23" width="10.5703125" style="14" customWidth="1"/>
-    <col min="24" max="16384" width="8.85546875" style="14"/>
+    <col min="1" max="5" width="10.54296875" style="13" customWidth="1"/>
+    <col min="6" max="23" width="10.54296875" style="14" customWidth="1"/>
+    <col min="24" max="16384" width="8.81640625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="W1" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+    <row r="2" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="68"/>
-      <c r="L2" s="68"/>
-      <c r="M2" s="68"/>
-      <c r="N2" s="68"/>
-      <c r="O2" s="68"/>
-      <c r="P2" s="68"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="68"/>
-      <c r="U2" s="68"/>
-      <c r="V2" s="68"/>
-      <c r="W2" s="68"/>
-    </row>
-    <row r="3" spans="1:23" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69" t="s">
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="91"/>
+      <c r="Q2" s="91"/>
+      <c r="R2" s="91"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="91"/>
+      <c r="U2" s="91"/>
+      <c r="V2" s="91"/>
+      <c r="W2" s="91"/>
+    </row>
+    <row r="3" spans="1:23" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
       <c r="I3" s="16"/>
       <c r="J3" s="16"/>
       <c r="K3" s="16"/>
@@ -2016,17 +2005,17 @@
       <c r="V3" s="16"/>
       <c r="W3" s="16"/>
     </row>
-    <row r="4" spans="1:23" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="69" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
+    <row r="4" spans="1:23" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="92" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="92"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
       <c r="I4" s="16"/>
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
@@ -2043,19 +2032,19 @@
       <c r="V4" s="16"/>
       <c r="W4" s="16"/>
     </row>
-    <row r="5" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-    </row>
-    <row r="6" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="92" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="102"/>
+      <c r="H5" s="102"/>
+    </row>
+    <row r="6" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="18"/>
       <c r="B6" s="18"/>
       <c r="C6" s="18"/>
@@ -2064,141 +2053,141 @@
       <c r="F6" s="18"/>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
+    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="93" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="C7" s="96"/>
+      <c r="D7" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="72" t="s">
+      <c r="E7" s="99"/>
+      <c r="F7" s="99"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="96"/>
+      <c r="N7" s="95" t="s">
+        <v>73</v>
+      </c>
+      <c r="O7" s="96"/>
+      <c r="P7" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="76"/>
-      <c r="L7" s="76"/>
-      <c r="M7" s="73"/>
-      <c r="N7" s="72" t="s">
-        <v>74</v>
-      </c>
-      <c r="O7" s="73"/>
-      <c r="P7" s="72" t="s">
+      <c r="Q7" s="99"/>
+      <c r="R7" s="96"/>
+      <c r="S7" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="73"/>
-      <c r="S7" s="72" t="s">
+      <c r="T7" s="96"/>
+      <c r="U7" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="T7" s="73"/>
-      <c r="U7" s="72" t="s">
+      <c r="V7" s="99"/>
+      <c r="W7" s="96"/>
+    </row>
+    <row r="8" spans="1:23" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="94"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="97"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82"/>
+      <c r="H8" s="82"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="82"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="98"/>
+      <c r="N8" s="97"/>
+      <c r="O8" s="98"/>
+      <c r="P8" s="97"/>
+      <c r="Q8" s="82"/>
+      <c r="R8" s="98"/>
+      <c r="S8" s="97"/>
+      <c r="T8" s="98"/>
+      <c r="U8" s="97"/>
+      <c r="V8" s="82"/>
+      <c r="W8" s="98"/>
+    </row>
+    <row r="9" spans="1:23" ht="320.14999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="94"/>
+      <c r="B9" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="V7" s="76"/>
-      <c r="W7" s="73"/>
-    </row>
-    <row r="8" spans="1:23" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="71"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
-      <c r="K8" s="77"/>
-      <c r="L8" s="77"/>
-      <c r="M8" s="75"/>
-      <c r="N8" s="74"/>
-      <c r="O8" s="75"/>
-      <c r="P8" s="74"/>
-      <c r="Q8" s="77"/>
-      <c r="R8" s="75"/>
-      <c r="S8" s="74"/>
-      <c r="T8" s="75"/>
-      <c r="U8" s="74"/>
-      <c r="V8" s="77"/>
-      <c r="W8" s="75"/>
-    </row>
-    <row r="9" spans="1:23" ht="320.10000000000002" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="71"/>
-      <c r="B9" s="19" t="s">
+      <c r="C9" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="D9" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="E9" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="F9" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="G9" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="H9" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="I9" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="J9" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="K9" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="K9" s="20" t="s">
+      <c r="L9" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="L9" s="20" t="s">
+      <c r="M9" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="M9" s="20" t="s">
+      <c r="N9" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="N9" s="20" t="s">
+      <c r="O9" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="O9" s="20" t="s">
+      <c r="P9" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="P9" s="20" t="s">
+      <c r="Q9" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="R9" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="S9" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="Q9" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="R9" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="S9" s="20" t="s">
+      <c r="T9" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="T9" s="20" t="s">
+      <c r="U9" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="U9" s="20" t="s">
-        <v>64</v>
-      </c>
       <c r="V9" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="W9" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="29">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="28">
         <v>1</v>
       </c>
       <c r="B10" s="22">
@@ -2268,7 +2257,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="15.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="21"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -2293,54 +2282,54 @@
       <c r="V11" s="21"/>
       <c r="W11" s="21"/>
     </row>
-    <row r="13" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="35" t="s">
+    <row r="14" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="C14" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="83" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="84"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="84"/>
-      <c r="I14" s="84"/>
-      <c r="J14" s="84"/>
-      <c r="K14" s="84"/>
-      <c r="L14" s="85"/>
-    </row>
-    <row r="15" spans="1:23" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="35"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="84"/>
-      <c r="L15" s="85"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="85"/>
+      <c r="L14" s="86"/>
+    </row>
+    <row r="15" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="32"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="85"/>
+      <c r="G15" s="85"/>
+      <c r="H15" s="85"/>
+      <c r="I15" s="85"/>
+      <c r="J15" s="85"/>
+      <c r="K15" s="85"/>
+      <c r="L15" s="86"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A16" s="23"/>
-      <c r="B16" s="86"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="87"/>
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
@@ -2350,69 +2339,60 @@
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="24"/>
-      <c r="B17" s="87"/>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="88"/>
+      <c r="D17" s="88"/>
       <c r="E17" s="24"/>
       <c r="F17" s="24"/>
-      <c r="G17" s="30"/>
+      <c r="G17" s="24"/>
       <c r="H17" s="24"/>
       <c r="I17" s="24"/>
       <c r="J17" s="24"/>
       <c r="K17" s="24"/>
       <c r="L17" s="24"/>
     </row>
-    <row r="18" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="88" t="s">
+    <row r="18" spans="1:12" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="89" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="82"/>
+      <c r="G18" s="82"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="82"/>
+      <c r="L18" s="82"/>
+    </row>
+    <row r="19" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="88"/>
-      <c r="C18" s="88"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="77"/>
-      <c r="G18" s="77"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="30"/>
-      <c r="K18" s="77"/>
-      <c r="L18" s="77"/>
-    </row>
-    <row r="19" spans="1:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="26" t="s">
+      <c r="E19" s="29"/>
+      <c r="F19" s="81" t="s">
         <v>70</v>
-      </c>
-      <c r="E19" s="31"/>
-      <c r="F19" s="81" t="s">
-        <v>71</v>
       </c>
       <c r="G19" s="81"/>
       <c r="H19" s="26"/>
       <c r="I19" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="J19" s="26"/>
+      <c r="K19" s="83" t="s">
         <v>72</v>
       </c>
-      <c r="J19" s="26"/>
-      <c r="K19" s="82" t="s">
-        <v>73</v>
-      </c>
-      <c r="L19" s="82"/>
+      <c r="L19" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="C14:L14"/>
-    <mergeCell ref="C15:L15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="F18:G18"/>
     <mergeCell ref="A2:W2"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:F4"/>
@@ -2427,6 +2407,15 @@
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="U7:W8"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="C14:L14"/>
+    <mergeCell ref="C15:L15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="F18:G18"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="53" fitToHeight="1000" orientation="landscape" r:id="rId1"/>

</xml_diff>